<commit_message>
added dblib, rf&transfrmrs xlsx
</commit_message>
<xml_diff>
--- a/library/digital.xlsx
+++ b/library/digital.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\elem_altium_db2\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1900E54-28D9-405F-8330-CCCBB5B4C285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B81C54-7C65-4FB2-89F8-A37628F6EAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="6705" windowWidth="21600" windowHeight="8670" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
+    <workbookView xWindow="9105" yWindow="1950" windowWidth="18705" windowHeight="10440" activeTab="5" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
@@ -527,13 +527,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent 3 2" xfId="1" xr:uid="{07D6D35A-A25D-4183-ACA2-756DA14CBAEA}"/>
@@ -851,11 +848,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67671D6E-5D55-4C0C-9FE7-A86F937C6875}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -966,10 +971,17 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1085,10 +1097,18 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1120,30 +1140,31 @@
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1158,21 +1179,22 @@
       <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1181,55 +1203,60 @@
       <c r="F4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1241,18 +1268,19 @@
       <c r="E7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1264,18 +1292,19 @@
       <c r="E8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1287,41 +1316,43 @@
       <c r="E9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1333,18 +1364,19 @@
       <c r="E11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1362,6 +1394,7 @@
       <c r="G12" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="H12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,7 +1411,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1533,10 +1570,18 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1849,13 +1894,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B396063C-A3E8-4F0D-BBD3-83031D2833E6}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>